<commit_message>
Update data and charts
</commit_message>
<xml_diff>
--- a/data/Laptop.xlsx
+++ b/data/Laptop.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,37 +463,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DELL G15 Intel Core i5 13th Gen 13450HX - (16 GB/1 TB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 3050/120 Hz) G15 5530 Gaming Laptop (15.6 Inch, Dark Shadow Gray With Black Thermal Shelf, 2.65 Kg, With MS Office)</t>
+          <t>Acer Aspire 7 Intel Core 5 210H - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 4050) A715-79G Gaming Laptop (15.6 Inch, Obsidian Black, 1.99 Kg)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>85990</v>
+        <v>69990</v>
       </c>
       <c r="C2" t="n">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Intel Core i5 13th Gen</t>
+          <t>Intel Core 5</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1 TB</t>
+          <t>512 GB</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Acer Aspire 7 Intel Core 5 210H - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 4050) A715-79G Gaming Laptop (15.6 Inch, Obsidian Black, 1.99 Kg)</t>
+          <t>Acer NITRO V 16S Intel Core 5 - (16 GB/512 GB SSD/Windows 11 Home/8 GB Graphics/NVIDIA GeForce RTX NVIDIA GeForce RTX 5050/180 Hz) ANV16S-71 Gaming Laptop (16 Inch, Obsidian Black, 2.1 kg)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>69990</v>
+        <v>94990</v>
       </c>
       <c r="C3" t="n">
-        <v>4.3</v>
+        <v>4.8</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -509,18 +509,18 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Acer NITRO LITE 16 Intel Core i5 13th Gen 13420H - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 3050) NL16-71G Gaming Laptop (16 Inch, Pure White, 1.95 Kg)</t>
+          <t>Lenovo LOQ Essential Intel Core i5 12th Gen 12450HX - (16 GB/512 GB SSD/Windows 11 Home/4 GB Graphics/NVIDIA GeForce RTX 3050A) 15IAX9E Gaming Laptop (15.6 Inch, Luna Grey, 1.77 kg, With MS Office)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>59990</v>
+        <v>68980</v>
       </c>
       <c r="C4" t="n">
-        <v>4.5</v>
+        <v>3.9</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Intel Core i5 13th Gen</t>
+          <t>Intel Core i5 12th Gen</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -532,18 +532,18 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Lenovo LOQ Essential Intel Core i5 12th Gen 12450HX - (16 GB/512 GB SSD/Windows 11 Home/4 GB Graphics/NVIDIA GeForce RTX 3050A) 15IAX9E Gaming Laptop (15.6 Inch, Luna Grey, 1.77 kg, With MS Office)</t>
+          <t>ASUS TUF Gaming A15 (2025) AMD Ryzen 7 Hexa Core 7445HS - (16 GB/512 GB SSD/Windows 11 Home/4 GB Graphics/NVIDIA GeForce RTX 3050/144 Hz) FA506NCG-HN199W Gaming Laptop (15.6 Inch, Graphite Black, 2.3 Kg)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>68980</v>
+        <v>72990</v>
       </c>
       <c r="C5" t="n">
-        <v>3.9</v>
+        <v>4.4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Intel Core i5 12th Gen</t>
+          <t>AMD Ryzen 7 Hexa Core</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -555,18 +555,18 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Acer NITRO V 16S Intel Core 5 - (16 GB/512 GB SSD/Windows 11 Home/8 GB Graphics/NVIDIA GeForce RTX NVIDIA GeForce RTX 5050/180 Hz) ANV16S-71 Gaming Laptop (16 Inch, Obsidian Black, 2.1 kg)</t>
+          <t>DELL G15 Intel Core i5 13th Gen 13450HX - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 3050/120 Hz) 5530 Gaming Laptop (15.6 Inch, Dark Shadow Gray With Black Thermal Shelf, 2.65 Kg, With MS Office)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>94990</v>
+        <v>79990</v>
       </c>
       <c r="C6" t="n">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Intel Core 5</t>
+          <t>Intel Core i5 13th Gen</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -578,37 +578,37 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Lenovo LOQ 2025 Intel Core i7 14th Gen 14700HX - (16 GB/1 TB SSD/Windows 11 Home/8 GB Graphics/NVIDIA GeForce RTX 5050) LoQ 15IRX10 Gaming Laptop (15.6 Inch, Luna Grey, 2.4 Kg, With MS Office)</t>
+          <t>Acer Aspire 7 Intel Core i7 13th Gen 13620H - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 4050) A715-79G Gaming Laptop (15.6 Inch, Obsidian Black, 1.99 Kg)</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>125990</v>
+        <v>84990</v>
       </c>
       <c r="C7" t="n">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Intel Core i7 14th Gen</t>
+          <t>Intel Core i7 13th Gen</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1 TB</t>
+          <t>512 GB</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DELL G15 Intel Core i5 13th Gen 13450HX - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 3050/120 Hz) 5530 Gaming Laptop (15.6 Inch, Dark Shadow Gray With Black Thermal Shelf, 2.65 Kg, With MS Office)</t>
+          <t>Lenovo LOQ Intel Core i5 13th Gen 13450HX - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 3050) LOQ 15IRX9D2 Gaming Laptop (15.6 Inch, Luna Grey, 2.38 kg, With MS Office)</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>79990</v>
+        <v>78990</v>
       </c>
       <c r="C8" t="n">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -624,41 +624,41 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Lenovo LOQ Essential Intel Core i7 12650HX - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 4050) LOQ 15IAX9E Gaming Laptop (15.6 Inch, Luna Grey, With MS Office)</t>
+          <t>HP Victus AMD Ryzen 7 Octa Core 260 - (24 GB/1 TB SSD/Windows 11 Home/8 GB Graphics/NVIDIA GeForce RTX 5050) 15-fb3185AX Gaming Laptop (15.6 Inch, Mica Silver, Black Chrome Logo, 2.29 Kg, With MS Office)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>79990</v>
+        <v>99990</v>
       </c>
       <c r="C9" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Intel Core i7</t>
+          <t>AMD Ryzen 7 Octa Core</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>512 GB</t>
+          <t>1 TB</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Acer Aspire 7 Intel Core i7 13th Gen 13620H - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 4050) A715-79G Gaming Laptop (15.6 Inch, Obsidian Black, 1.99 Kg)</t>
+          <t>HP Victus AMD Ryzen 7 Hexa Core 7445HS - (16 GB/512 GB SSD/Windows 11 Home/4 GB Graphics/NVIDIA GeForce RTX 2050) 15-fb3122AX Gaming Laptop (15.6 Inch, Performance Blue, Chrome Logo, 2.29 Kg, With MS Office)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>84990</v>
+        <v>63990</v>
       </c>
       <c r="C10" t="n">
-        <v>4.2</v>
+        <v>4.4</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Intel Core i7 13th Gen</t>
+          <t>AMD Ryzen 7 Hexa Core</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -670,41 +670,41 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HP Victus AMD Ryzen 7 Hexa Core 7445HS - (16 GB/512 GB SSD/Windows 11 Home/4 GB Graphics/NVIDIA GeForce RTX 2050) 15-fb3122AX Gaming Laptop (15.6 Inch, Performance Blue, Chrome Logo, 2.29 Kg, With MS Office)</t>
+          <t>Lenovo LOQ 2025 Intel Core i7 13th Gen 13700HX - (16 GB/1 TB SSD/Windows 11 Home/8 GB Graphics/NVIDIA GeForce RTX 5060) LoQ 15IRX10 Gaming Laptop (15.6 Inch, Luna Grey, 2.4 Kg, With MS Office)</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>63990</v>
+        <v>127990</v>
       </c>
       <c r="C11" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>AMD Ryzen 7 Hexa Core</t>
+          <t>Intel Core i7 13th Gen</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>512 GB</t>
+          <t>1 TB</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Acer Nitro V AMD Ryzen 5 Hexa Core 6600H - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 3050) ANV15-41-R8G0 Gaming Laptop (16 Inch, Obsidian Black, 2.1 Kg)</t>
+          <t>Acer Aspire 7 Intel Core i5 13th Gen 13420H - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 3050) A715-79G Gaming Laptop (15.6 Inch, Black, 1.99 Kg)</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>62990</v>
       </c>
       <c r="C12" t="n">
-        <v>4.4</v>
+        <v>4.3</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>AMD Ryzen 5 Hexa Core</t>
+          <t>Intel Core i5 13th Gen</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -716,136 +716,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HP Victus Intel Core i5 14th Gen 14450HX - (24 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 4050) 15-fa2382TX Gaming Laptop (15.6 Inch, Mica Silver, 2.31 Kg, With MS Office)</t>
+          <t>Lenovo LOQ Intel Core i5 13th Gen 13450HX - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 4050) 15IRX9 Gaming Laptop (15.6 Inch, Luna Grey, 2.38 Kg, With MS Office)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>89990</v>
+        <v>87990</v>
       </c>
       <c r="C13" t="n">
-        <v>4.3</v>
+        <v>4.4</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Intel Core i5 14th Gen</t>
+          <t>Intel Core i5 13th Gen</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
-        <is>
-          <t>512 GB</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Lenovo LOQ AMD Ryzen 7 Octa Core 7435HS - (24 GB/512 GB SSD/Windows 11 Home/4 GB Graphics/NVIDIA GeForce RTX 3050A) LOQ 15ARP9D2 Gaming Laptop (15.6 Inch, Luna Grey, 2.38 kg, With MS Office)</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>71290</v>
-      </c>
-      <c r="C14" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>AMD Ryzen 7 Octa Core</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>512 GB</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Lenovo LOQ 2025 Intel Core i7 13th Gen 13700HX - (16 GB/1 TB SSD/Windows 11 Home/8 GB Graphics/NVIDIA GeForce RTX 5060) LoQ 15IRX10 Gaming Laptop (15.6 Inch, Luna Grey, 2.4 Kg, With MS Office)</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>127990</v>
-      </c>
-      <c r="C15" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Intel Core i7 13th Gen</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>1 TB</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Lenovo IdeaPad Slim 3 AMD Ryzen 7 Octa Core - (16 GB/512 GB SSD/Windows 11 Home) IdeaPad Slim 3 15AHP10 Thin and Light Laptop (15.3 Inch, Luna Grey, 1.59 kg, With MS Office)</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>67390</v>
-      </c>
-      <c r="C16" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>AMD Ryzen 7 Octa Core</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>512 GB</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Acer Aspire 7 Intel Core i5 13th Gen 13420H - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 3050) A715-79G Gaming Laptop (15.6 Inch, Black, 1.99 Kg)</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>62990</v>
-      </c>
-      <c r="C17" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Intel Core i5 13th Gen</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>512 GB</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Lenovo LOQ Intel Core i5 13th Gen 13450HX - (16 GB/512 GB SSD/Windows 11 Home/6 GB Graphics/NVIDIA GeForce RTX 4050) 15IRX9 Gaming Laptop (15.6 Inch, Luna Grey, 2.38 Kg, With MS Office)</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>87990</v>
-      </c>
-      <c r="C18" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Intel Core i5 13th Gen</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
         <is>
           <t>512 GB</t>
         </is>

</xml_diff>